<commit_message>
Bug fixes. Stat Changes. Space Saving.
-Changed the way items are selected to save space.
-Adjusted stat values to feel better.
-Weapons and Armor are now multiples of 3 to be more impactful to the game.
-First NPC encounter gives hint for the map.
</commit_message>
<xml_diff>
--- a/maths/DamageCalculator.xlsx
+++ b/maths/DamageCalculator.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11790" windowHeight="13660" xr2:uid="{129A14B1-4A38-4FD3-B06A-76EA20AB62F9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11793" windowHeight="13660" xr2:uid="{129A14B1-4A38-4FD3-B06A-76EA20AB62F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
   <si>
     <t>Player</t>
   </si>
@@ -77,12 +77,21 @@
   <si>
     <t>PlayerFaster?</t>
   </si>
+  <si>
+    <t>Player Bonuses</t>
+  </si>
+  <si>
+    <t>Attack:</t>
+  </si>
+  <si>
+    <t>Defense:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,8 +106,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +140,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -130,12 +159,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,17 +484,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17747D8-1842-4355-8AD6-D06F6DFB8FDD}">
   <dimension ref="A1:T48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="14" max="14" width="5.1796875" customWidth="1"/>
-    <col min="15" max="15" width="11.54296875" customWidth="1"/>
+    <col min="14" max="14" width="5.17578125" customWidth="1"/>
+    <col min="15" max="15" width="11.52734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,7 +502,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -508,7 +540,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -540,7 +572,7 @@
       </c>
       <c r="J3">
         <f>(H3*$J$46)+($J$48*(H3-1))</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K3">
         <f>(H3*$K$46)+($K$48*(H3-1))</f>
@@ -555,13 +587,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:B42" si="0">$B$48+((A4-1)*$B$46)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C42" si="1">$C$48+((A4-1)*$C$46)</f>
@@ -573,7 +605,7 @@
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E42" si="3">$E$48+((A4-1)*$E$46)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F4">
         <f t="shared" ref="F4:F42" si="4">$F$48+((A4-1)*$F$46)</f>
@@ -588,7 +620,7 @@
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J42" si="6">(H4*$J$46)+($J$48*(H4-1))</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K42" si="7">(H4*$K$46)+($K$48*(H4-1))</f>
@@ -603,13 +635,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
@@ -621,7 +653,7 @@
       </c>
       <c r="E5">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F5">
         <f t="shared" si="4"/>
@@ -636,28 +668,28 @@
       </c>
       <c r="J5">
         <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="7"/>
+      <c r="L5">
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
-      <c r="L5">
-        <f t="shared" si="8"/>
-        <v>9</v>
-      </c>
       <c r="M5">
         <f t="shared" si="9"/>
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
@@ -669,7 +701,7 @@
       </c>
       <c r="E6">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F6">
         <f t="shared" si="4"/>
@@ -684,7 +716,7 @@
       </c>
       <c r="J6">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="K6">
         <f t="shared" si="7"/>
@@ -702,13 +734,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
@@ -720,7 +752,7 @@
       </c>
       <c r="E7">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F7">
         <f t="shared" si="4"/>
@@ -735,7 +767,7 @@
       </c>
       <c r="J7">
         <f t="shared" si="6"/>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="K7">
         <f t="shared" si="7"/>
@@ -765,13 +797,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
@@ -783,7 +815,7 @@
       </c>
       <c r="E8">
         <f t="shared" si="3"/>
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F8">
         <f t="shared" si="4"/>
@@ -798,7 +830,7 @@
       </c>
       <c r="J8">
         <f t="shared" si="6"/>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="K8">
         <f t="shared" si="7"/>
@@ -816,32 +848,32 @@
         <v>0</v>
       </c>
       <c r="P8">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="Q8">
         <f>INDEX(B3:B42,P8)</f>
-        <v>26</v>
+        <v>153</v>
       </c>
       <c r="R8">
-        <f>INDEX(D3:D42,P8)</f>
-        <v>8</v>
+        <f>INDEX(D3:D42,P8)+P20</f>
+        <v>86</v>
       </c>
       <c r="S8">
         <f>INDEX(E3:E42,P8)</f>
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="T8">
         <f>INDEX(F3:F42,P8)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
@@ -853,7 +885,7 @@
       </c>
       <c r="E9">
         <f t="shared" si="3"/>
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F9">
         <f t="shared" si="4"/>
@@ -868,7 +900,7 @@
       </c>
       <c r="J9">
         <f t="shared" si="6"/>
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="K9">
         <f t="shared" si="7"/>
@@ -886,32 +918,32 @@
         <v>9</v>
       </c>
       <c r="P9">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="Q9">
         <f>INDEX(I3:I42,P9)</f>
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="R9">
-        <f>INDEX(J3:J42,P9)</f>
-        <v>3</v>
+        <f>INDEX(J3:J42,P9)+P21</f>
+        <v>144</v>
       </c>
       <c r="S9">
         <f>INDEX(K3:K42,P9)</f>
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="T9">
         <f>INDEX(M3:M42,P9)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
@@ -923,7 +955,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="3"/>
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="F10">
         <f t="shared" si="4"/>
@@ -938,7 +970,7 @@
       </c>
       <c r="J10">
         <f t="shared" si="6"/>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="K10">
         <f t="shared" si="7"/>
@@ -959,13 +991,13 @@
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
@@ -977,7 +1009,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="3"/>
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="F11">
         <f t="shared" si="4"/>
@@ -992,7 +1024,7 @@
       </c>
       <c r="J11">
         <f t="shared" si="6"/>
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="K11">
         <f t="shared" si="7"/>
@@ -1010,17 +1042,17 @@
         <v>13</v>
       </c>
       <c r="P11" s="2">
-        <f>FLOOR(MAX(R8/S9*P8, 1),1)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+        <f>FLOOR(MAX(P8*R8/S9, 1),1)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
@@ -1032,7 +1064,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="F12">
         <f t="shared" si="4"/>
@@ -1047,7 +1079,7 @@
       </c>
       <c r="J12">
         <f t="shared" si="6"/>
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="K12">
         <f t="shared" si="7"/>
@@ -1066,16 +1098,16 @@
       </c>
       <c r="P12" s="2">
         <f>CEILING(Q9/P11,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
@@ -1087,7 +1119,7 @@
       </c>
       <c r="E13">
         <f t="shared" si="3"/>
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="F13">
         <f t="shared" si="4"/>
@@ -1102,7 +1134,7 @@
       </c>
       <c r="J13">
         <f t="shared" si="6"/>
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="K13">
         <f t="shared" si="7"/>
@@ -1122,13 +1154,13 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
@@ -1140,7 +1172,7 @@
       </c>
       <c r="E14">
         <f t="shared" si="3"/>
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="F14">
         <f t="shared" si="4"/>
@@ -1155,7 +1187,7 @@
       </c>
       <c r="J14">
         <f t="shared" si="6"/>
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="K14">
         <f t="shared" si="7"/>
@@ -1173,17 +1205,17 @@
         <v>13</v>
       </c>
       <c r="P14" s="4">
-        <f>FLOOR(MAX(R9/S8*P8, 1),1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+        <f>FLOOR(MAX(P8*R9/S8, 1),1)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
@@ -1195,7 +1227,7 @@
       </c>
       <c r="E15">
         <f t="shared" si="3"/>
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="F15">
         <f t="shared" si="4"/>
@@ -1210,7 +1242,7 @@
       </c>
       <c r="J15">
         <f t="shared" si="6"/>
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="K15">
         <f t="shared" si="7"/>
@@ -1229,16 +1261,16 @@
       </c>
       <c r="P15" s="4">
         <f>CEILING(Q8/P14,1)</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
@@ -1250,7 +1282,7 @@
       </c>
       <c r="E16">
         <f t="shared" si="3"/>
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="F16">
         <f t="shared" si="4"/>
@@ -1265,28 +1297,28 @@
       </c>
       <c r="J16">
         <f t="shared" si="6"/>
+        <v>84</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="7"/>
         <v>42</v>
       </c>
-      <c r="K16">
-        <f t="shared" si="7"/>
+      <c r="L16">
+        <f t="shared" si="8"/>
         <v>42</v>
       </c>
-      <c r="L16">
-        <f t="shared" si="8"/>
-        <v>42</v>
-      </c>
       <c r="M16">
         <f t="shared" si="9"/>
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
@@ -1298,7 +1330,7 @@
       </c>
       <c r="E17">
         <f t="shared" si="3"/>
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F17">
         <f t="shared" si="4"/>
@@ -1313,7 +1345,7 @@
       </c>
       <c r="J17">
         <f t="shared" si="6"/>
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="K17">
         <f t="shared" si="7"/>
@@ -1332,16 +1364,16 @@
       </c>
       <c r="P17" t="b">
         <f>T8&gt;T9</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
@@ -1353,7 +1385,7 @@
       </c>
       <c r="E18">
         <f t="shared" si="3"/>
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="F18">
         <f t="shared" si="4"/>
@@ -1368,28 +1400,28 @@
       </c>
       <c r="J18">
         <f t="shared" si="6"/>
+        <v>96</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
-      <c r="K18">
-        <f t="shared" si="7"/>
+      <c r="L18">
+        <f t="shared" si="8"/>
         <v>48</v>
       </c>
-      <c r="L18">
-        <f t="shared" si="8"/>
-        <v>48</v>
-      </c>
       <c r="M18">
         <f t="shared" si="9"/>
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
@@ -1401,7 +1433,7 @@
       </c>
       <c r="E19">
         <f t="shared" si="3"/>
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="F19">
         <f t="shared" si="4"/>
@@ -1416,28 +1448,32 @@
       </c>
       <c r="J19">
         <f t="shared" si="6"/>
+        <v>102</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="7"/>
         <v>51</v>
       </c>
-      <c r="K19">
-        <f t="shared" si="7"/>
+      <c r="L19">
+        <f t="shared" si="8"/>
         <v>51</v>
       </c>
-      <c r="L19">
-        <f t="shared" si="8"/>
-        <v>51</v>
-      </c>
       <c r="M19">
         <f t="shared" si="9"/>
         <v>85</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P19" s="7"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
@@ -1449,7 +1485,7 @@
       </c>
       <c r="E20">
         <f t="shared" si="3"/>
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="F20">
         <f t="shared" si="4"/>
@@ -1464,28 +1500,34 @@
       </c>
       <c r="J20">
         <f t="shared" si="6"/>
+        <v>108</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="7"/>
         <v>54</v>
       </c>
-      <c r="K20">
-        <f t="shared" si="7"/>
+      <c r="L20">
+        <f t="shared" si="8"/>
         <v>54</v>
       </c>
-      <c r="L20">
-        <f t="shared" si="8"/>
-        <v>54</v>
-      </c>
       <c r="M20">
         <f t="shared" si="9"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P20" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
@@ -1497,7 +1539,7 @@
       </c>
       <c r="E21">
         <f t="shared" si="3"/>
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="F21">
         <f t="shared" si="4"/>
@@ -1512,28 +1554,34 @@
       </c>
       <c r="J21">
         <f t="shared" si="6"/>
+        <v>114</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="7"/>
         <v>57</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="7"/>
+      <c r="L21">
+        <f t="shared" si="8"/>
         <v>57</v>
       </c>
-      <c r="L21">
-        <f t="shared" si="8"/>
-        <v>57</v>
-      </c>
       <c r="M21">
         <f t="shared" si="9"/>
         <v>95</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P21" s="6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
@@ -1545,7 +1593,7 @@
       </c>
       <c r="E22">
         <f t="shared" si="3"/>
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="F22">
         <f t="shared" si="4"/>
@@ -1560,28 +1608,28 @@
       </c>
       <c r="J22">
         <f t="shared" si="6"/>
+        <v>120</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
-      <c r="K22">
-        <f t="shared" si="7"/>
+      <c r="L22">
+        <f t="shared" si="8"/>
         <v>60</v>
       </c>
-      <c r="L22">
-        <f t="shared" si="8"/>
-        <v>60</v>
-      </c>
       <c r="M22">
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
@@ -1593,7 +1641,7 @@
       </c>
       <c r="E23">
         <f t="shared" si="3"/>
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="F23">
         <f t="shared" si="4"/>
@@ -1608,28 +1656,28 @@
       </c>
       <c r="J23">
         <f t="shared" si="6"/>
+        <v>126</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="7"/>
         <v>63</v>
       </c>
-      <c r="K23">
-        <f t="shared" si="7"/>
+      <c r="L23">
+        <f t="shared" si="8"/>
         <v>63</v>
       </c>
-      <c r="L23">
-        <f t="shared" si="8"/>
-        <v>63</v>
-      </c>
       <c r="M23">
         <f t="shared" si="9"/>
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
@@ -1641,7 +1689,7 @@
       </c>
       <c r="E24">
         <f t="shared" si="3"/>
-        <v>91</v>
+        <v>133</v>
       </c>
       <c r="F24">
         <f t="shared" si="4"/>
@@ -1656,28 +1704,28 @@
       </c>
       <c r="J24">
         <f t="shared" si="6"/>
+        <v>132</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="7"/>
         <v>66</v>
       </c>
-      <c r="K24">
-        <f t="shared" si="7"/>
+      <c r="L24">
+        <f t="shared" si="8"/>
         <v>66</v>
       </c>
-      <c r="L24">
-        <f t="shared" si="8"/>
-        <v>66</v>
-      </c>
       <c r="M24">
         <f t="shared" si="9"/>
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
@@ -1689,7 +1737,7 @@
       </c>
       <c r="E25">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="F25">
         <f t="shared" si="4"/>
@@ -1704,28 +1752,28 @@
       </c>
       <c r="J25">
         <f t="shared" si="6"/>
+        <v>138</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="7"/>
         <v>69</v>
       </c>
-      <c r="K25">
-        <f t="shared" si="7"/>
+      <c r="L25">
+        <f t="shared" si="8"/>
         <v>69</v>
       </c>
-      <c r="L25">
-        <f t="shared" si="8"/>
-        <v>69</v>
-      </c>
       <c r="M25">
         <f t="shared" si="9"/>
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
@@ -1737,7 +1785,7 @@
       </c>
       <c r="E26">
         <f t="shared" si="3"/>
-        <v>99</v>
+        <v>145</v>
       </c>
       <c r="F26">
         <f t="shared" si="4"/>
@@ -1752,28 +1800,28 @@
       </c>
       <c r="J26">
         <f t="shared" si="6"/>
+        <v>144</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="7"/>
         <v>72</v>
       </c>
-      <c r="K26">
-        <f t="shared" si="7"/>
+      <c r="L26">
+        <f t="shared" si="8"/>
         <v>72</v>
       </c>
-      <c r="L26">
-        <f t="shared" si="8"/>
-        <v>72</v>
-      </c>
       <c r="M26">
         <f t="shared" si="9"/>
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
@@ -1785,7 +1833,7 @@
       </c>
       <c r="E27">
         <f t="shared" si="3"/>
-        <v>103</v>
+        <v>151</v>
       </c>
       <c r="F27">
         <f t="shared" si="4"/>
@@ -1800,28 +1848,28 @@
       </c>
       <c r="J27">
         <f t="shared" si="6"/>
+        <v>150</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="7"/>
         <v>75</v>
       </c>
-      <c r="K27">
-        <f t="shared" si="7"/>
+      <c r="L27">
+        <f t="shared" si="8"/>
         <v>75</v>
       </c>
-      <c r="L27">
-        <f t="shared" si="8"/>
-        <v>75</v>
-      </c>
       <c r="M27">
         <f t="shared" si="9"/>
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
@@ -1833,7 +1881,7 @@
       </c>
       <c r="E28">
         <f t="shared" si="3"/>
-        <v>107</v>
+        <v>157</v>
       </c>
       <c r="F28">
         <f t="shared" si="4"/>
@@ -1848,28 +1896,28 @@
       </c>
       <c r="J28">
         <f t="shared" si="6"/>
+        <v>156</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="7"/>
         <v>78</v>
       </c>
-      <c r="K28">
-        <f t="shared" si="7"/>
+      <c r="L28">
+        <f t="shared" si="8"/>
         <v>78</v>
       </c>
-      <c r="L28">
-        <f t="shared" si="8"/>
-        <v>78</v>
-      </c>
       <c r="M28">
         <f t="shared" si="9"/>
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
@@ -1881,7 +1929,7 @@
       </c>
       <c r="E29">
         <f t="shared" si="3"/>
-        <v>111</v>
+        <v>163</v>
       </c>
       <c r="F29">
         <f t="shared" si="4"/>
@@ -1896,28 +1944,28 @@
       </c>
       <c r="J29">
         <f t="shared" si="6"/>
+        <v>162</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="7"/>
         <v>81</v>
       </c>
-      <c r="K29">
-        <f t="shared" si="7"/>
+      <c r="L29">
+        <f t="shared" si="8"/>
         <v>81</v>
       </c>
-      <c r="L29">
-        <f t="shared" si="8"/>
-        <v>81</v>
-      </c>
       <c r="M29">
         <f t="shared" si="9"/>
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
@@ -1929,7 +1977,7 @@
       </c>
       <c r="E30">
         <f t="shared" si="3"/>
-        <v>115</v>
+        <v>169</v>
       </c>
       <c r="F30">
         <f t="shared" si="4"/>
@@ -1944,28 +1992,28 @@
       </c>
       <c r="J30">
         <f t="shared" si="6"/>
+        <v>168</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="7"/>
         <v>84</v>
       </c>
-      <c r="K30">
-        <f t="shared" si="7"/>
+      <c r="L30">
+        <f t="shared" si="8"/>
         <v>84</v>
       </c>
-      <c r="L30">
-        <f t="shared" si="8"/>
-        <v>84</v>
-      </c>
       <c r="M30">
         <f t="shared" si="9"/>
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>188</v>
+        <v>216</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
@@ -1977,7 +2025,7 @@
       </c>
       <c r="E31">
         <f t="shared" si="3"/>
-        <v>119</v>
+        <v>175</v>
       </c>
       <c r="F31">
         <f t="shared" si="4"/>
@@ -1992,28 +2040,28 @@
       </c>
       <c r="J31">
         <f t="shared" si="6"/>
+        <v>174</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="7"/>
         <v>87</v>
       </c>
-      <c r="K31">
-        <f t="shared" si="7"/>
+      <c r="L31">
+        <f t="shared" si="8"/>
         <v>87</v>
       </c>
-      <c r="L31">
-        <f t="shared" si="8"/>
-        <v>87</v>
-      </c>
       <c r="M31">
         <f t="shared" si="9"/>
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>194</v>
+        <v>223</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
@@ -2025,7 +2073,7 @@
       </c>
       <c r="E32">
         <f t="shared" si="3"/>
-        <v>123</v>
+        <v>181</v>
       </c>
       <c r="F32">
         <f t="shared" si="4"/>
@@ -2040,28 +2088,28 @@
       </c>
       <c r="J32">
         <f t="shared" si="6"/>
+        <v>180</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="7"/>
         <v>90</v>
       </c>
-      <c r="K32">
-        <f t="shared" si="7"/>
+      <c r="L32">
+        <f t="shared" si="8"/>
         <v>90</v>
       </c>
-      <c r="L32">
-        <f t="shared" si="8"/>
-        <v>90</v>
-      </c>
       <c r="M32">
         <f t="shared" si="9"/>
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
@@ -2073,7 +2121,7 @@
       </c>
       <c r="E33">
         <f t="shared" si="3"/>
-        <v>127</v>
+        <v>187</v>
       </c>
       <c r="F33">
         <f t="shared" si="4"/>
@@ -2088,28 +2136,28 @@
       </c>
       <c r="J33">
         <f t="shared" si="6"/>
+        <v>186</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="7"/>
         <v>93</v>
       </c>
-      <c r="K33">
-        <f t="shared" si="7"/>
+      <c r="L33">
+        <f t="shared" si="8"/>
         <v>93</v>
       </c>
-      <c r="L33">
-        <f t="shared" si="8"/>
-        <v>93</v>
-      </c>
       <c r="M33">
         <f t="shared" si="9"/>
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>206</v>
+        <v>237</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
@@ -2121,7 +2169,7 @@
       </c>
       <c r="E34">
         <f t="shared" si="3"/>
-        <v>131</v>
+        <v>193</v>
       </c>
       <c r="F34">
         <f t="shared" si="4"/>
@@ -2136,28 +2184,28 @@
       </c>
       <c r="J34">
         <f t="shared" si="6"/>
+        <v>192</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="7"/>
         <v>96</v>
       </c>
-      <c r="K34">
-        <f t="shared" si="7"/>
+      <c r="L34">
+        <f t="shared" si="8"/>
         <v>96</v>
       </c>
-      <c r="L34">
-        <f t="shared" si="8"/>
-        <v>96</v>
-      </c>
       <c r="M34">
         <f t="shared" si="9"/>
         <v>160</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>212</v>
+        <v>244</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
@@ -2169,7 +2217,7 @@
       </c>
       <c r="E35">
         <f t="shared" si="3"/>
-        <v>135</v>
+        <v>199</v>
       </c>
       <c r="F35">
         <f t="shared" si="4"/>
@@ -2184,28 +2232,28 @@
       </c>
       <c r="J35">
         <f t="shared" si="6"/>
+        <v>198</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="7"/>
         <v>99</v>
       </c>
-      <c r="K35">
-        <f t="shared" si="7"/>
+      <c r="L35">
+        <f t="shared" si="8"/>
         <v>99</v>
       </c>
-      <c r="L35">
-        <f t="shared" si="8"/>
-        <v>99</v>
-      </c>
       <c r="M35">
         <f t="shared" si="9"/>
         <v>165</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
@@ -2217,7 +2265,7 @@
       </c>
       <c r="E36">
         <f t="shared" si="3"/>
-        <v>139</v>
+        <v>205</v>
       </c>
       <c r="F36">
         <f t="shared" si="4"/>
@@ -2232,28 +2280,28 @@
       </c>
       <c r="J36">
         <f t="shared" si="6"/>
+        <v>204</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="7"/>
         <v>102</v>
       </c>
-      <c r="K36">
-        <f t="shared" si="7"/>
+      <c r="L36">
+        <f t="shared" si="8"/>
         <v>102</v>
       </c>
-      <c r="L36">
-        <f t="shared" si="8"/>
-        <v>102</v>
-      </c>
       <c r="M36">
         <f t="shared" si="9"/>
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>224</v>
+        <v>258</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
@@ -2265,7 +2313,7 @@
       </c>
       <c r="E37">
         <f t="shared" si="3"/>
-        <v>143</v>
+        <v>211</v>
       </c>
       <c r="F37">
         <f t="shared" si="4"/>
@@ -2280,28 +2328,28 @@
       </c>
       <c r="J37">
         <f t="shared" si="6"/>
+        <v>210</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="7"/>
         <v>105</v>
       </c>
-      <c r="K37">
-        <f t="shared" si="7"/>
+      <c r="L37">
+        <f t="shared" si="8"/>
         <v>105</v>
       </c>
-      <c r="L37">
-        <f t="shared" si="8"/>
-        <v>105</v>
-      </c>
       <c r="M37">
         <f t="shared" si="9"/>
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>230</v>
+        <v>265</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
@@ -2313,7 +2361,7 @@
       </c>
       <c r="E38">
         <f t="shared" si="3"/>
-        <v>147</v>
+        <v>217</v>
       </c>
       <c r="F38">
         <f t="shared" si="4"/>
@@ -2328,28 +2376,28 @@
       </c>
       <c r="J38">
         <f t="shared" si="6"/>
+        <v>216</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="7"/>
         <v>108</v>
       </c>
-      <c r="K38">
-        <f t="shared" si="7"/>
+      <c r="L38">
+        <f t="shared" si="8"/>
         <v>108</v>
       </c>
-      <c r="L38">
-        <f t="shared" si="8"/>
-        <v>108</v>
-      </c>
       <c r="M38">
         <f t="shared" si="9"/>
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>236</v>
+        <v>272</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
@@ -2361,7 +2409,7 @@
       </c>
       <c r="E39">
         <f t="shared" si="3"/>
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="F39">
         <f t="shared" si="4"/>
@@ -2376,28 +2424,28 @@
       </c>
       <c r="J39">
         <f t="shared" si="6"/>
+        <v>222</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="7"/>
         <v>111</v>
       </c>
-      <c r="K39">
-        <f t="shared" si="7"/>
+      <c r="L39">
+        <f t="shared" si="8"/>
         <v>111</v>
       </c>
-      <c r="L39">
-        <f t="shared" si="8"/>
-        <v>111</v>
-      </c>
       <c r="M39">
         <f t="shared" si="9"/>
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>242</v>
+        <v>279</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
@@ -2409,7 +2457,7 @@
       </c>
       <c r="E40">
         <f t="shared" si="3"/>
-        <v>155</v>
+        <v>229</v>
       </c>
       <c r="F40">
         <f t="shared" si="4"/>
@@ -2424,28 +2472,28 @@
       </c>
       <c r="J40">
         <f t="shared" si="6"/>
+        <v>228</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="7"/>
         <v>114</v>
       </c>
-      <c r="K40">
-        <f t="shared" si="7"/>
+      <c r="L40">
+        <f t="shared" si="8"/>
         <v>114</v>
       </c>
-      <c r="L40">
-        <f t="shared" si="8"/>
-        <v>114</v>
-      </c>
       <c r="M40">
         <f t="shared" si="9"/>
         <v>190</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>248</v>
+        <v>286</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
@@ -2457,7 +2505,7 @@
       </c>
       <c r="E41">
         <f t="shared" si="3"/>
-        <v>159</v>
+        <v>235</v>
       </c>
       <c r="F41">
         <f t="shared" si="4"/>
@@ -2472,28 +2520,28 @@
       </c>
       <c r="J41">
         <f t="shared" si="6"/>
+        <v>234</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="7"/>
         <v>117</v>
       </c>
-      <c r="K41">
-        <f t="shared" si="7"/>
+      <c r="L41">
+        <f t="shared" si="8"/>
         <v>117</v>
       </c>
-      <c r="L41">
-        <f t="shared" si="8"/>
-        <v>117</v>
-      </c>
       <c r="M41">
         <f t="shared" si="9"/>
         <v>195</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>254</v>
+        <v>293</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
@@ -2505,7 +2553,7 @@
       </c>
       <c r="E42">
         <f t="shared" si="3"/>
-        <v>163</v>
+        <v>241</v>
       </c>
       <c r="F42">
         <f t="shared" si="4"/>
@@ -2520,22 +2568,22 @@
       </c>
       <c r="J42">
         <f t="shared" si="6"/>
+        <v>240</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="7"/>
         <v>120</v>
       </c>
-      <c r="K42">
-        <f t="shared" si="7"/>
+      <c r="L42">
+        <f t="shared" si="8"/>
         <v>120</v>
       </c>
-      <c r="L42">
-        <f t="shared" si="8"/>
-        <v>120</v>
-      </c>
       <c r="M42">
         <f t="shared" si="9"/>
         <v>200</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -2573,9 +2621,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B46">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C46">
         <v>6</v>
@@ -2584,7 +2632,7 @@
         <v>3</v>
       </c>
       <c r="E46">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F46">
         <v>5</v>
@@ -2593,7 +2641,7 @@
         <v>3</v>
       </c>
       <c r="J46">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K46">
         <v>3</v>
@@ -2605,7 +2653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -2643,7 +2691,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B48">
         <v>20</v>
       </c>
@@ -2677,5 +2725,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>